<commit_message>
Data file and login page locators added.
</commit_message>
<xml_diff>
--- a/Excel_Data/test_data.xlsx
+++ b/Excel_Data/test_data.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Animesh_Mukherjee\PycharmProjects\Demo_WebShop_POM\Excel_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BABE5CE4-867F-4836-B943-4264583A0918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CEF2B3C-0428-4793-9D82-DCC734F8A22E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="login_test" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -394,7 +394,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Verify product review test added.
</commit_message>
<xml_diff>
--- a/Excel_Data/test_data.xlsx
+++ b/Excel_Data/test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Animesh_Mukherjee\PycharmProjects\Demo_WebShop_POM\Excel_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A032F1-38CB-4C1B-9E19-959E1C624A86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC38616-B990-4597-A9E9-ACD7789E2E10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -408,7 +408,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Search product review test added.
</commit_message>
<xml_diff>
--- a/Excel_Data/test_data.xlsx
+++ b/Excel_Data/test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Animesh_Mukherjee\PycharmProjects\Demo_WebShop_POM\Excel_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903919C0-DB65-4E93-AFDE-C4E0CBF23D0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D96D1E-5788-4204-84B5-8727CE6577B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>admin@yourstore.com</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>created_to_date</t>
+  </si>
+  <si>
+    <t>1/1/2017</t>
+  </si>
+  <si>
+    <t>11/15/2021</t>
   </si>
 </sst>
 </file>
@@ -117,7 +123,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -403,7 +409,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -435,11 +441,11 @@
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3">
-        <v>42736</v>
-      </c>
-      <c r="D2" s="3">
-        <v>44541</v>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>